<commit_message>
resulting files of bioblitz 2019
</commit_message>
<xml_diff>
--- a/01_spreadsheet/results/bioblitz_2019_Brown.xlsx
+++ b/01_spreadsheet/results/bioblitz_2019_Brown.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">PTM1979</t>
   </si>
   <si>
+    <t xml:space="preserve">PTM1981</t>
+  </si>
+  <si>
     <t xml:space="preserve">PTM1982</t>
   </si>
   <si>
@@ -233,6 +236,15 @@
     <t xml:space="preserve">Alana Breitkreutz</t>
   </si>
   <si>
+    <t xml:space="preserve">Elachistaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elachista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elachista fucicola</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laminariaceae</t>
   </si>
   <si>
@@ -402,6 +414,9 @@
   </si>
   <si>
     <t xml:space="preserve">low/mid intertidal on boulder with Ulva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low intertidal, epiphytic on Fucus</t>
   </si>
   <si>
     <t xml:space="preserve">Low intertidal to shallow subtidal</t>
@@ -993,6 +1008,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1012,40 +1042,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
@@ -1053,32 +1083,32 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -1092,32 +1122,32 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -1131,32 +1161,32 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
@@ -1170,32 +1200,32 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
@@ -1209,32 +1239,32 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
         <v>6</v>
@@ -1248,32 +1278,32 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
@@ -1287,32 +1317,32 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
         <v>6</v>
@@ -1326,32 +1356,32 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L9" t="s">
         <v>6</v>
@@ -1365,32 +1395,32 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J10" t="s">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" t="s">
         <v>6</v>
@@ -1404,32 +1434,32 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s">
         <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L11" t="s">
         <v>6</v>
@@ -1443,32 +1473,32 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
         <v>6</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L12" t="s">
         <v>6</v>
@@ -1482,32 +1512,32 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L13" t="s">
         <v>6</v>
@@ -1521,32 +1551,32 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
       </c>
       <c r="K14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L14" t="s">
         <v>6</v>
@@ -1560,32 +1590,32 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J15" t="s">
         <v>6</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L15" t="s">
         <v>6</v>
@@ -1599,32 +1629,32 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J16" t="s">
         <v>6</v>
       </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L16" t="s">
         <v>6</v>
@@ -1638,37 +1668,76 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J17" t="s">
         <v>6</v>
       </c>
       <c r="K17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L17" t="s">
         <v>6</v>
       </c>
       <c r="M17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1691,34 +1760,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
@@ -2246,6 +2315,39 @@
         <v>6</v>
       </c>
       <c r="K17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2268,70 +2370,70 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="N1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="Q1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="R1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="S1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="T1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="U1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="V1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="W1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -2342,28 +2444,28 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -2390,7 +2492,7 @@
         <v>6</v>
       </c>
       <c r="S2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="T2" t="s">
         <v>6</v>
@@ -2413,28 +2515,28 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K3" t="s">
         <v>6</v>
@@ -2461,7 +2563,7 @@
         <v>6</v>
       </c>
       <c r="S3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="T3" t="s">
         <v>6</v>
@@ -2484,28 +2586,28 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
@@ -2532,7 +2634,7 @@
         <v>6</v>
       </c>
       <c r="S4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="T4" t="s">
         <v>6</v>
@@ -2555,28 +2657,28 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -2603,7 +2705,7 @@
         <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="T5" t="s">
         <v>6</v>
@@ -2626,28 +2728,28 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -2674,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="S6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="T6" t="s">
         <v>6</v>
@@ -2697,28 +2799,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K7" t="s">
         <v>6</v>
@@ -2745,7 +2847,7 @@
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="T7" t="s">
         <v>6</v>
@@ -2768,28 +2870,28 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K8" t="s">
         <v>6</v>
@@ -2816,7 +2918,7 @@
         <v>6</v>
       </c>
       <c r="S8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="T8" t="s">
         <v>6</v>
@@ -2839,28 +2941,28 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
@@ -2887,7 +2989,7 @@
         <v>6</v>
       </c>
       <c r="S9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="T9" t="s">
         <v>6</v>
@@ -2910,28 +3012,28 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I10" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K10" t="s">
         <v>6</v>
@@ -2958,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="S10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="T10" t="s">
         <v>6</v>
@@ -2981,28 +3083,28 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K11" t="s">
         <v>6</v>
@@ -3029,7 +3131,7 @@
         <v>6</v>
       </c>
       <c r="S11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T11" t="s">
         <v>6</v>
@@ -3052,28 +3154,28 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I12" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K12" t="s">
         <v>6</v>
@@ -3100,7 +3202,7 @@
         <v>6</v>
       </c>
       <c r="S12" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="T12" t="s">
         <v>6</v>
@@ -3123,28 +3225,28 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H13" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I13" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>
@@ -3171,7 +3273,7 @@
         <v>6</v>
       </c>
       <c r="S13" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T13" t="s">
         <v>6</v>
@@ -3194,28 +3296,28 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H14" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I14" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J14" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
@@ -3242,7 +3344,7 @@
         <v>6</v>
       </c>
       <c r="S14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T14" t="s">
         <v>6</v>
@@ -3265,28 +3367,28 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H15" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I15" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J15" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K15" t="s">
         <v>6</v>
@@ -3313,7 +3415,7 @@
         <v>6</v>
       </c>
       <c r="S15" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T15" t="s">
         <v>6</v>
@@ -3336,28 +3438,28 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J16" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K16" t="s">
         <v>6</v>
@@ -3384,7 +3486,7 @@
         <v>6</v>
       </c>
       <c r="S16" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T16" t="s">
         <v>6</v>
@@ -3407,28 +3509,28 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H17" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K17" t="s">
         <v>6</v>
@@ -3455,18 +3557,89 @@
         <v>6</v>
       </c>
       <c r="S17" t="s">
+        <v>133</v>
+      </c>
+      <c r="T17" t="s">
+        <v>6</v>
+      </c>
+      <c r="U17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" t="s">
+        <v>6</v>
+      </c>
+      <c r="W17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" t="s">
         <v>129</v>
       </c>
-      <c r="T17" t="s">
-        <v>6</v>
-      </c>
-      <c r="U17" t="s">
-        <v>6</v>
-      </c>
-      <c r="V17" t="s">
-        <v>6</v>
-      </c>
-      <c r="W17" t="s">
+      <c r="J18" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>6</v>
+      </c>
+      <c r="R18" t="s">
+        <v>6</v>
+      </c>
+      <c r="S18" t="s">
+        <v>134</v>
+      </c>
+      <c r="T18" t="s">
+        <v>6</v>
+      </c>
+      <c r="U18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" t="s">
+        <v>6</v>
+      </c>
+      <c r="W18" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>